<commit_message>
fitting to unisensory means
fitting with conditions defined as centered on the unisensory means rather than the actual target locations. Will see if this works at all better than previous version
</commit_message>
<xml_diff>
--- a/doc/writing_logs.xlsx
+++ b/doc/writing_logs.xlsx
@@ -371,10 +371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,6 +467,70 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43664</v>
+      </c>
+      <c r="B5" s="3">
+        <f>C4</f>
+        <v>5276</v>
+      </c>
+      <c r="C5" s="3">
+        <v>5445</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" ref="D5:D20" si="0">C5-B5</f>
+        <v>169</v>
+      </c>
+      <c r="E5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added improved lapse description
lapse unity now applies also to the localization trials. The major change here is that now the "lapse" trials are single saccades drawn from either of the unimodal distributions (with equal probability) rather than from the integrated distribution. This matches better with behavior, where the overwhelming number of inappropriate lapses occur when the monkey makes only one saccade to either of the targets, then gives up, even though the targets are obviously well separated.
</commit_message>
<xml_diff>
--- a/doc/writing_logs.xlsx
+++ b/doc/writing_logs.xlsx
@@ -374,7 +374,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,7 +479,7 @@
         <v>5445</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D20" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D6" si="0">C5-B5</f>
         <v>169</v>
       </c>
       <c r="E5">
@@ -487,7 +487,23 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D6" s="3"/>
+      <c r="A6" s="1">
+        <v>43669</v>
+      </c>
+      <c r="B6" s="3">
+        <f>C5</f>
+        <v>5445</v>
+      </c>
+      <c r="C6" s="3">
+        <v>5851</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="0"/>
+        <v>406</v>
+      </c>
+      <c r="E6">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D7" s="3"/>

</xml_diff>

<commit_message>
state of project for first draft
</commit_message>
<xml_diff>
--- a/doc/writing_logs.xlsx
+++ b/doc/writing_logs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11880"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,18 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>date</t>
   </si>
@@ -48,6 +54,9 @@
   </si>
   <si>
     <t>638 words of this are from the references, but I'm going to just leave that in cause otherwise I have to subtract references all the time.</t>
+  </si>
+  <si>
+    <t>removed all outline text. a lot of edits were made the previous two days (7/29 and 7/30) and not recorded. This is pretty much the end of my first draft stage</t>
   </si>
 </sst>
 </file>
@@ -374,7 +383,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,7 +488,7 @@
         <v>5445</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D6" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D9" si="0">C5-B5</f>
         <v>169</v>
       </c>
       <c r="E5">
@@ -506,13 +515,64 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D7" s="3"/>
+      <c r="A7" s="1">
+        <v>43671</v>
+      </c>
+      <c r="B7" s="3">
+        <f>C6</f>
+        <v>5851</v>
+      </c>
+      <c r="C7" s="3">
+        <v>7414</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="0"/>
+        <v>1563</v>
+      </c>
+      <c r="E7">
+        <v>2.25</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D8" s="3"/>
+      <c r="A8" s="1">
+        <v>43672</v>
+      </c>
+      <c r="B8" s="3">
+        <f>C7</f>
+        <v>7414</v>
+      </c>
+      <c r="C8" s="3">
+        <v>7693</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="0"/>
+        <v>279</v>
+      </c>
+      <c r="E8">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D9" s="3"/>
+      <c r="A9" s="1">
+        <v>43677</v>
+      </c>
+      <c r="B9" s="3">
+        <f>C8</f>
+        <v>7693</v>
+      </c>
+      <c r="C9" s="3">
+        <v>7082</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>-611</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D10" s="3"/>

</xml_diff>